<commit_message>
Update menus with additional traj macros
</commit_message>
<xml_diff>
--- a/FRC_LV_Trajectory_Library/Misc/FRC_LabVIEW_Trajectory_Library_Routines.xlsx
+++ b/FRC_LV_Trajectory_Library/Misc/FRC_LabVIEW_Trajectory_Library_Routines.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7460" uniqueCount="1562">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7483" uniqueCount="1565">
   <si>
     <t xml:space="preserve">FRC LabVIEW Trajectory Library – VI Implementation List</t>
   </si>
@@ -4447,7 +4447,7 @@
     <t xml:space="preserve">EXTENDED_KALMAN_CORRECT_FUNC_GROUP.CTL</t>
   </si>
   <si>
-    <t xml:space="preserve">ExTENDED_KALMAN_FILTER.CTL</t>
+    <t xml:space="preserve">EXTENDED_KALMAN_FILTER.CTL</t>
   </si>
   <si>
     <t xml:space="preserve">FLYWHEEL_SIM.ctl</t>
@@ -4633,13 +4633,22 @@
     <t xml:space="preserve">TRAJ_CONSTRAINT_DIIF_DRIVE_VOLTAGE.CTL</t>
   </si>
   <si>
+    <t xml:space="preserve">TRAJ_CONSTRAINT_ELLIP_REGION.CTL</t>
+  </si>
+  <si>
     <t xml:space="preserve">TRAJ_CONSTRAINT_JERK.CTL</t>
   </si>
   <si>
+    <t xml:space="preserve">TRAJ_CONSTRAINT_MAX_VELOCITY.CTL</t>
+  </si>
+  <si>
     <t xml:space="preserve">TRAJ_CONSTRAINT_MECA_DRIVE_KINEMATICS.CTL</t>
   </si>
   <si>
     <t xml:space="preserve">TRAJ_CONSTRAINT_MINMAX.CTL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAJ_CONSTRAINT_RECT_REGION.CTL</t>
   </si>
   <si>
     <t xml:space="preserve">TRAJ_CONSTRAINT_SWERVE_DRIVE_KINEMATICS.CTL</t>
@@ -5103,22 +5112,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -5187,10 +5180,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:AMI1048576"/>
+  <dimension ref="A1:AMI1551"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A761" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A764" activeCellId="0" sqref="A764"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5300,35 +5293,35 @@
       </c>
       <c r="B9" s="13" t="n">
         <f aca="false">B10+B11</f>
-        <v>1066</v>
+        <v>1069</v>
       </c>
       <c r="C9" s="13" t="n">
-        <f aca="false">COUNTIF(C21:C1874,"X")</f>
+        <f aca="false">COUNTIF(C21:C1877,"X")</f>
         <v>1010</v>
       </c>
       <c r="D9" s="13" t="n">
-        <f aca="false">COUNTIF(D21:D1874,"X")</f>
-        <v>328</v>
+        <f aca="false">COUNTIF(D21:D1877,"X")</f>
+        <v>331</v>
       </c>
       <c r="E9" s="13" t="n">
-        <f aca="false">COUNTIF(E21:E1874,"X")</f>
-        <v>1005</v>
+        <f aca="false">COUNTIF(E21:E1877,"X")</f>
+        <v>1016</v>
       </c>
       <c r="F9" s="13" t="n">
-        <f aca="false">COUNTIF(F21:F1874,"S")+COUNTIF(F21:F1874,"I")+COUNTIF(F21:F1874,"X")+COUNTIF(F21:F1874,"SI")+COUNTIF(F21:F1874,"IS")+COUNTIF(F21:F1874,"N/A")</f>
-        <v>596</v>
+        <f aca="false">COUNTIF(F21:F1877,"S")+COUNTIF(F21:F1877,"I")+COUNTIF(F21:F1877,"X")+COUNTIF(F21:F1877,"SI")+COUNTIF(F21:F1877,"IS")+COUNTIF(F21:F1877,"N/A")</f>
+        <v>599</v>
       </c>
       <c r="G9" s="13" t="n">
-        <f aca="false">COUNTIF(G21:G1874,"S")+COUNTIF(G21:G1874,"I")+COUNTIF(G21:G1874,"X")+COUNTIF(G21:G1874,"SI")+COUNTIF(G21:G1874,"IS")+COUNTIF(G21:G1874,"N/A")</f>
+        <f aca="false">COUNTIF(G21:G1877,"S")+COUNTIF(G21:G1877,"I")+COUNTIF(G21:G1877,"X")+COUNTIF(G21:G1877,"SI")+COUNTIF(G21:G1877,"IS")+COUNTIF(G21:G1877,"N/A")</f>
         <v>51</v>
       </c>
       <c r="H9" s="13" t="n">
-        <f aca="false">COUNTIF(H21:H1874,"S")+COUNTIF(H21:H1874,"I")+COUNTIF(H21:H1874,"X")+COUNTIF(H21:H1874,"SI")+COUNTIF(H21:H1874,"IS")+COUNTIF(H21:H1874,"N/A")</f>
+        <f aca="false">COUNTIF(H21:H1877,"S")+COUNTIF(H21:H1877,"I")+COUNTIF(H21:H1877,"X")+COUNTIF(H21:H1877,"SI")+COUNTIF(H21:H1877,"IS")+COUNTIF(H21:H1877,"N/A")</f>
         <v>12</v>
       </c>
       <c r="I9" s="14" t="n">
         <f aca="false">C9/B9</f>
-        <v>0.947467166979362</v>
+        <v>0.944808231992516</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5336,7 +5329,7 @@
         <v>14</v>
       </c>
       <c r="B10" s="13" t="n">
-        <f aca="false">COUNTIF(B21:B1874,"X")</f>
+        <f aca="false">COUNTIF(B21:B1877,"X")</f>
         <v>958</v>
       </c>
       <c r="I10" s="3" t="s">
@@ -5348,12 +5341,12 @@
         <v>16</v>
       </c>
       <c r="B11" s="13" t="n">
-        <f aca="false">COUNTIF(B21:B1874,"Z")</f>
-        <v>108</v>
+        <f aca="false">COUNTIF(B21:B1877,"Z")</f>
+        <v>111</v>
       </c>
       <c r="I11" s="15" t="n">
         <f aca="false">F9/B9</f>
-        <v>0.559099437148218</v>
+        <v>0.560336763330215</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5361,7 +5354,7 @@
         <v>17</v>
       </c>
       <c r="B12" s="13" t="n">
-        <f aca="false">COUNTIF(B21:B1874,"/")</f>
+        <f aca="false">COUNTIF(B21:B1877,"/")</f>
         <v>4</v>
       </c>
       <c r="I12" s="4"/>
@@ -5371,7 +5364,7 @@
         <v>18</v>
       </c>
       <c r="B13" s="13" t="n">
-        <f aca="false">COUNTIF(B21:B1874,"\")</f>
+        <f aca="false">COUNTIF(B21:B1877,"\")</f>
         <v>2</v>
       </c>
       <c r="I13" s="4" t="s">
@@ -21319,7 +21312,9 @@
         <v>30</v>
       </c>
       <c r="D636" s="22"/>
-      <c r="E636" s="26"/>
+      <c r="E636" s="22" t="s">
+        <v>30</v>
+      </c>
       <c r="F636" s="22"/>
       <c r="G636" s="22"/>
       <c r="H636" s="22"/>
@@ -21395,7 +21390,9 @@
       <c r="D639" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="E639" s="26"/>
+      <c r="E639" s="22" t="s">
+        <v>30</v>
+      </c>
       <c r="F639" s="22"/>
       <c r="G639" s="22"/>
       <c r="H639" s="22"/>
@@ -21419,7 +21416,9 @@
       </c>
       <c r="C640" s="26"/>
       <c r="D640" s="22"/>
-      <c r="E640" s="26"/>
+      <c r="E640" s="22" t="s">
+        <v>30</v>
+      </c>
       <c r="F640" s="22"/>
       <c r="G640" s="22"/>
       <c r="H640" s="22"/>
@@ -21511,7 +21510,9 @@
       <c r="D644" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="E644" s="26"/>
+      <c r="E644" s="22" t="s">
+        <v>30</v>
+      </c>
       <c r="F644" s="22"/>
       <c r="G644" s="22"/>
       <c r="H644" s="22"/>
@@ -21531,7 +21532,9 @@
       </c>
       <c r="C645" s="26"/>
       <c r="D645" s="22"/>
-      <c r="E645" s="26"/>
+      <c r="E645" s="22" t="s">
+        <v>30</v>
+      </c>
       <c r="F645" s="22"/>
       <c r="G645" s="22"/>
       <c r="H645" s="22"/>
@@ -21577,7 +21580,9 @@
       </c>
       <c r="C647" s="26"/>
       <c r="D647" s="22"/>
-      <c r="E647" s="26"/>
+      <c r="E647" s="22" t="s">
+        <v>30</v>
+      </c>
       <c r="F647" s="22"/>
       <c r="G647" s="22"/>
       <c r="H647" s="22"/>
@@ -21629,7 +21634,9 @@
       </c>
       <c r="C649" s="26"/>
       <c r="D649" s="22"/>
-      <c r="E649" s="26"/>
+      <c r="E649" s="22" t="s">
+        <v>30</v>
+      </c>
       <c r="F649" s="22"/>
       <c r="G649" s="22"/>
       <c r="H649" s="22"/>
@@ -21763,7 +21770,9 @@
       </c>
       <c r="C654" s="26"/>
       <c r="D654" s="22"/>
-      <c r="E654" s="26"/>
+      <c r="E654" s="22" t="s">
+        <v>30</v>
+      </c>
       <c r="F654" s="22"/>
       <c r="G654" s="22"/>
       <c r="H654" s="22"/>
@@ -43075,14 +43084,16 @@
     </row>
     <row r="1525" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1525" s="9"/>
-      <c r="B1525" s="28" t="s">
-        <v>1445</v>
+      <c r="B1525" s="22" t="s">
+        <v>1442</v>
       </c>
       <c r="C1525" s="26"/>
       <c r="D1525" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="E1525" s="26"/>
+      <c r="E1525" s="22" t="s">
+        <v>30</v>
+      </c>
       <c r="F1525" s="22" t="s">
         <v>890</v>
       </c>
@@ -43092,24 +43103,18 @@
         <v>1536</v>
       </c>
       <c r="J1525" s="23"/>
-      <c r="K1525" s="23" t="s">
-        <v>850</v>
-      </c>
+      <c r="K1525" s="23"/>
     </row>
     <row r="1526" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1526" s="9"/>
-      <c r="B1526" s="22" t="s">
-        <v>1442</v>
-      </c>
-      <c r="C1526" s="22" t="s">
-        <v>30</v>
-      </c>
+      <c r="B1526" s="28" t="s">
+        <v>1445</v>
+      </c>
+      <c r="C1526" s="26"/>
       <c r="D1526" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="E1526" s="22" t="s">
-        <v>30</v>
-      </c>
+      <c r="E1526" s="26"/>
       <c r="F1526" s="22" t="s">
         <v>890</v>
       </c>
@@ -43119,16 +43124,16 @@
         <v>1537</v>
       </c>
       <c r="J1526" s="23"/>
-      <c r="K1526" s="23"/>
+      <c r="K1526" s="23" t="s">
+        <v>850</v>
+      </c>
     </row>
     <row r="1527" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1527" s="9"/>
       <c r="B1527" s="22" t="s">
         <v>1442</v>
       </c>
-      <c r="C1527" s="22" t="s">
-        <v>30</v>
-      </c>
+      <c r="C1527" s="26"/>
       <c r="D1527" s="22" t="s">
         <v>30</v>
       </c>
@@ -43196,14 +43201,12 @@
       <c r="J1529" s="23"/>
       <c r="K1529" s="23"/>
     </row>
-    <row r="1530" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1530" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1530" s="9"/>
       <c r="B1530" s="22" t="s">
         <v>1442</v>
       </c>
-      <c r="C1530" s="22" t="s">
-        <v>30</v>
-      </c>
+      <c r="C1530" s="26"/>
       <c r="D1530" s="22" t="s">
         <v>30</v>
       </c>
@@ -43271,7 +43274,7 @@
       <c r="J1532" s="23"/>
       <c r="K1532" s="23"/>
     </row>
-    <row r="1533" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1533" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1533" s="9"/>
       <c r="B1533" s="22" t="s">
         <v>1442</v>
@@ -43297,6 +43300,7 @@
       <c r="K1533" s="23"/>
     </row>
     <row r="1534" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1534" s="9"/>
       <c r="B1534" s="22" t="s">
         <v>1442</v>
       </c>
@@ -43321,6 +43325,7 @@
       <c r="K1534" s="23"/>
     </row>
     <row r="1535" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1535" s="9"/>
       <c r="B1535" s="22" t="s">
         <v>1442</v>
       </c>
@@ -43344,7 +43349,8 @@
       <c r="J1535" s="23"/>
       <c r="K1535" s="23"/>
     </row>
-    <row r="1536" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1536" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1536" s="9"/>
       <c r="B1536" s="22" t="s">
         <v>1442</v>
       </c>
@@ -43368,7 +43374,7 @@
       <c r="J1536" s="23"/>
       <c r="K1536" s="23"/>
     </row>
-    <row r="1537" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1537" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1537" s="22" t="s">
         <v>1442</v>
       </c>
@@ -43392,7 +43398,7 @@
       <c r="J1537" s="23"/>
       <c r="K1537" s="23"/>
     </row>
-    <row r="1538" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1538" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1538" s="22" t="s">
         <v>1442</v>
       </c>
@@ -43416,7 +43422,7 @@
       <c r="J1538" s="23"/>
       <c r="K1538" s="23"/>
     </row>
-    <row r="1539" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1539" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1539" s="22" t="s">
         <v>1442</v>
       </c>
@@ -43440,7 +43446,7 @@
       <c r="J1539" s="23"/>
       <c r="K1539" s="23"/>
     </row>
-    <row r="1540" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1540" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1540" s="22" t="s">
         <v>1442</v>
       </c>
@@ -43488,7 +43494,7 @@
       <c r="J1541" s="23"/>
       <c r="K1541" s="23"/>
     </row>
-    <row r="1542" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1542" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1542" s="22" t="s">
         <v>1442</v>
       </c>
@@ -43512,7 +43518,7 @@
       <c r="J1542" s="23"/>
       <c r="K1542" s="23"/>
     </row>
-    <row r="1543" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1543" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1543" s="22" t="s">
         <v>1442</v>
       </c>
@@ -43536,7 +43542,7 @@
       <c r="J1543" s="23"/>
       <c r="K1543" s="23"/>
     </row>
-    <row r="1544" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1544" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1544" s="22" t="s">
         <v>1442</v>
       </c>
@@ -43560,27 +43566,29 @@
       <c r="J1544" s="23"/>
       <c r="K1544" s="23"/>
     </row>
-    <row r="1545" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1545" s="28" t="s">
+    <row r="1545" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1545" s="22" t="s">
+        <v>1442</v>
+      </c>
+      <c r="C1545" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1545" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1545" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1545" s="22" t="s">
         <v>890</v>
       </c>
-      <c r="C1545" s="28"/>
-      <c r="D1545" s="28" t="s">
-        <v>890</v>
-      </c>
-      <c r="E1545" s="28"/>
-      <c r="F1545" s="28" t="s">
-        <v>890</v>
-      </c>
-      <c r="G1545" s="28"/>
-      <c r="H1545" s="28"/>
-      <c r="I1545" s="29" t="s">
+      <c r="G1545" s="22"/>
+      <c r="H1545" s="22"/>
+      <c r="I1545" s="23" t="s">
         <v>1556</v>
       </c>
-      <c r="J1545" s="29"/>
-      <c r="K1545" s="29" t="s">
-        <v>1557</v>
-      </c>
+      <c r="J1545" s="23"/>
+      <c r="K1545" s="23"/>
     </row>
     <row r="1546" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1546" s="22" t="s">
@@ -43596,67 +43604,134 @@
         <v>30</v>
       </c>
       <c r="F1546" s="22" t="s">
-        <v>1466</v>
+        <v>890</v>
       </c>
       <c r="G1546" s="22"/>
       <c r="H1546" s="22"/>
       <c r="I1546" s="23" t="s">
+        <v>1557</v>
+      </c>
+      <c r="J1546" s="23"/>
+      <c r="K1546" s="23"/>
+    </row>
+    <row r="1547" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1547" s="22" t="s">
+        <v>1442</v>
+      </c>
+      <c r="C1547" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1547" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1547" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1547" s="22" t="s">
+        <v>890</v>
+      </c>
+      <c r="G1547" s="22"/>
+      <c r="H1547" s="22"/>
+      <c r="I1547" s="23" t="s">
         <v>1558</v>
       </c>
-      <c r="J1546" s="23"/>
-      <c r="K1546" s="23" t="s">
+      <c r="J1547" s="23"/>
+      <c r="K1547" s="23"/>
+    </row>
+    <row r="1548" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1548" s="28" t="s">
+        <v>890</v>
+      </c>
+      <c r="C1548" s="28"/>
+      <c r="D1548" s="28" t="s">
+        <v>890</v>
+      </c>
+      <c r="E1548" s="28"/>
+      <c r="F1548" s="28" t="s">
+        <v>890</v>
+      </c>
+      <c r="G1548" s="28"/>
+      <c r="H1548" s="28"/>
+      <c r="I1548" s="29" t="s">
         <v>1559</v>
       </c>
-    </row>
-    <row r="1547" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1547" s="28" t="s">
+      <c r="J1548" s="29"/>
+      <c r="K1548" s="29" t="s">
+        <v>1560</v>
+      </c>
+    </row>
+    <row r="1549" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1549" s="22" t="s">
+        <v>1442</v>
+      </c>
+      <c r="C1549" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1549" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1549" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1549" s="22" t="s">
+        <v>1466</v>
+      </c>
+      <c r="G1549" s="22"/>
+      <c r="H1549" s="22"/>
+      <c r="I1549" s="23" t="s">
+        <v>1561</v>
+      </c>
+      <c r="J1549" s="23"/>
+      <c r="K1549" s="23" t="s">
+        <v>1562</v>
+      </c>
+    </row>
+    <row r="1550" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1550" s="28" t="s">
         <v>890</v>
       </c>
-      <c r="C1547" s="28"/>
-      <c r="D1547" s="28" t="s">
+      <c r="C1550" s="28"/>
+      <c r="D1550" s="28" t="s">
         <v>890</v>
       </c>
-      <c r="E1547" s="28"/>
-      <c r="F1547" s="28" t="s">
+      <c r="E1550" s="28"/>
+      <c r="F1550" s="28" t="s">
         <v>890</v>
       </c>
-      <c r="G1547" s="28"/>
-      <c r="H1547" s="28"/>
-      <c r="I1547" s="29" t="s">
+      <c r="G1550" s="28"/>
+      <c r="H1550" s="28"/>
+      <c r="I1550" s="29" t="s">
+        <v>1563</v>
+      </c>
+      <c r="J1550" s="29"/>
+      <c r="K1550" s="29" t="s">
         <v>1560</v>
       </c>
-      <c r="J1547" s="29"/>
-      <c r="K1547" s="29" t="s">
-        <v>1557</v>
-      </c>
-    </row>
-    <row r="1548" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1548" s="22" t="s">
+    </row>
+    <row r="1551" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1551" s="22" t="s">
         <v>1442</v>
       </c>
-      <c r="C1548" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1548" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1548" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="F1548" s="22" t="s">
+      <c r="C1551" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1551" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1551" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1551" s="22" t="s">
         <v>890</v>
       </c>
-      <c r="G1548" s="22"/>
-      <c r="H1548" s="22"/>
-      <c r="I1548" s="23" t="s">
-        <v>1561</v>
-      </c>
-      <c r="J1548" s="23"/>
-      <c r="K1548" s="23"/>
-    </row>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="G1551" s="22"/>
+      <c r="H1551" s="22"/>
+      <c r="I1551" s="23" t="s">
+        <v>1564</v>
+      </c>
+      <c r="J1551" s="23"/>
+      <c r="K1551" s="23"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.766666666666667" header="0.511811023622047" footer="0.5"/>

</xml_diff>

<commit_message>
documentation updates for network udp routines.  Issue #115
</commit_message>
<xml_diff>
--- a/FRC_LV_Trajectory_Library/Misc/FRC_LabVIEW_Trajectory_Library_Routines.xlsx
+++ b/FRC_LV_Trajectory_Library/Misc/FRC_LabVIEW_Trajectory_Library_Routines.xlsx
@@ -23,12 +23,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7835" uniqueCount="1626">
-  <si>
-    <t xml:space="preserve">FRC LabVIEW Trajectory Library – VI Implementation List</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revision 2.X   11/06/2022 – added various routines</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7841" uniqueCount="1626">
+  <si>
+    <t xml:space="preserve">WPILib LabVIEW Math Library – VI Implementation List</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revision 3.X   1/11/2023 – renamed library.  Added additional documentation.</t>
   </si>
   <si>
     <t xml:space="preserve">This documents which Java/C++ WPILIB routines have been </t>
@@ -5375,8 +5375,8 @@
   </sheetPr>
   <dimension ref="A1:AMI1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1595" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1625" activeCellId="0" sqref="E1625"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5490,7 +5490,7 @@
       </c>
       <c r="C9" s="13" t="n">
         <f aca="false">C10+C11</f>
-        <v>1098</v>
+        <v>1101</v>
       </c>
       <c r="D9" s="13" t="n">
         <f aca="false">COUNTIF(D24:D1948,"X")</f>
@@ -5502,7 +5502,7 @@
       </c>
       <c r="F9" s="13" t="n">
         <f aca="false">COUNTIF(F24:F1948,"S")+COUNTIF(F24:F1948,"I")+COUNTIF(F24:F1948,"X")+COUNTIF(F24:F1948,"SI")+COUNTIF(F24:F1948,"IS")+COUNTIF(F24:F1948,"N/A")</f>
-        <v>629</v>
+        <v>632</v>
       </c>
       <c r="G9" s="13" t="n">
         <f aca="false">COUNTIF(G24:G1948,"S")+COUNTIF(G24:G1948,"I")+COUNTIF(G24:G1948,"X")+COUNTIF(G24:G1948,"SI")+COUNTIF(G24:G1948,"IS")+COUNTIF(G24:G1948,"N/A")</f>
@@ -5514,7 +5514,7 @@
       </c>
       <c r="I9" s="14" t="n">
         <f aca="false">C9/B9</f>
-        <v>0.990974729241877</v>
+        <v>0.993682310469314</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5527,7 +5527,7 @@
       </c>
       <c r="C10" s="13" t="n">
         <f aca="false">COUNTIF(C24:C1948,"X")</f>
-        <v>986</v>
+        <v>989</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>15</v>
@@ -5547,7 +5547,7 @@
       </c>
       <c r="I11" s="15" t="n">
         <f aca="false">F9/B9</f>
-        <v>0.567689530685921</v>
+        <v>0.570397111913357</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -42578,12 +42578,16 @@
       <c r="B1494" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="C1494" s="26"/>
+      <c r="C1494" s="22" t="s">
+        <v>30</v>
+      </c>
       <c r="D1494" s="22" t="s">
         <v>30</v>
       </c>
       <c r="E1494" s="26"/>
-      <c r="F1494" s="26"/>
+      <c r="F1494" s="22" t="s">
+        <v>40</v>
+      </c>
       <c r="G1494" s="22"/>
       <c r="H1494" s="22"/>
       <c r="I1494" s="23" t="s">
@@ -42601,12 +42605,16 @@
       <c r="B1495" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="C1495" s="26"/>
+      <c r="C1495" s="22" t="s">
+        <v>30</v>
+      </c>
       <c r="D1495" s="22" t="s">
         <v>30</v>
       </c>
       <c r="E1495" s="26"/>
-      <c r="F1495" s="26"/>
+      <c r="F1495" s="22" t="s">
+        <v>31</v>
+      </c>
       <c r="G1495" s="22"/>
       <c r="H1495" s="22"/>
       <c r="I1495" s="23" t="s">
@@ -42624,12 +42632,16 @@
       <c r="B1496" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="C1496" s="26"/>
+      <c r="C1496" s="22" t="s">
+        <v>30</v>
+      </c>
       <c r="D1496" s="22" t="s">
         <v>30</v>
       </c>
       <c r="E1496" s="26"/>
-      <c r="F1496" s="26"/>
+      <c r="F1496" s="22" t="s">
+        <v>31</v>
+      </c>
       <c r="G1496" s="22"/>
       <c r="H1496" s="22"/>
       <c r="I1496" s="23" t="s">

</xml_diff>

<commit_message>
Update menus for new things.  #147 #146 #144 #141 #139 #138 #137  #135 #134
</commit_message>
<xml_diff>
--- a/FRC_LV_Trajectory_Library/Misc/FRC_LabVIEW_Trajectory_Library_Routines.xlsx
+++ b/FRC_LV_Trajectory_Library/Misc/FRC_LabVIEW_Trajectory_Library_Routines.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10014" uniqueCount="1723">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10098" uniqueCount="1723">
   <si>
     <t xml:space="preserve">WPILib LabVIEW Math Library – VI Implementation List</t>
   </si>
@@ -1882,7 +1882,7 @@
     <t xml:space="preserve">Replacement for orig diff drive odom</t>
   </si>
   <si>
-    <t xml:space="preserve">DiffDrvOdom2_GetPosevi</t>
+    <t xml:space="preserve">DiffDrvOdom2_GetPose.vi</t>
   </si>
   <si>
     <t xml:space="preserve">DiffDrvOdom2_New.vi</t>
@@ -5600,6 +5600,64 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFDDDDDD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00CCFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFCC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF33FF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -5671,7 +5729,7 @@
   <dimension ref="A1:AMI1727"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="B47" activeCellId="0" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5785,7 +5843,7 @@
       </c>
       <c r="C9" s="13" t="n">
         <f aca="false">C10+C11</f>
-        <v>1165</v>
+        <v>1175</v>
       </c>
       <c r="D9" s="13" t="n">
         <f aca="false">COUNTIF(D24:D2053,"X")</f>
@@ -5793,7 +5851,7 @@
       </c>
       <c r="E9" s="13" t="n">
         <f aca="false">COUNTIF(E24:E2053,"X")</f>
-        <v>1055</v>
+        <v>1119</v>
       </c>
       <c r="F9" s="13" t="n">
         <f aca="false">COUNTIF(F24:F2053,"S")+COUNTIF(F24:F2053,"I")+COUNTIF(F24:F2053,"X")+COUNTIF(F24:F2053,"SI")+COUNTIF(F24:F2053,"IS")+COUNTIF(F24:F2053,"N/A")</f>
@@ -5809,7 +5867,7 @@
       </c>
       <c r="I9" s="14" t="n">
         <f aca="false">C9/B9</f>
-        <v>0.977348993288591</v>
+        <v>0.985738255033557</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5822,7 +5880,7 @@
       </c>
       <c r="C10" s="13" t="n">
         <f aca="false">COUNTIF(C24:C2053,"X")</f>
-        <v>1046</v>
+        <v>1056</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>15</v>
@@ -6815,7 +6873,9 @@
         <v>32</v>
       </c>
       <c r="D47" s="23"/>
-      <c r="E47" s="28"/>
+      <c r="E47" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F47" s="23" t="s">
         <v>33</v>
       </c>
@@ -7992,7 +8052,9 @@
       <c r="D87" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="E87" s="28"/>
+      <c r="E87" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F87" s="28"/>
       <c r="G87" s="23"/>
       <c r="H87" s="23"/>
@@ -8295,7 +8357,9 @@
       <c r="D97" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="E97" s="28"/>
+      <c r="E97" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F97" s="23" t="s">
         <v>43</v>
       </c>
@@ -8403,7 +8467,9 @@
       <c r="D101" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="E101" s="28"/>
+      <c r="E101" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F101" s="23" t="s">
         <v>43</v>
       </c>
@@ -8621,7 +8687,9 @@
       <c r="D108" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="E108" s="28"/>
+      <c r="E108" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F108" s="23" t="s">
         <v>43</v>
       </c>
@@ -8679,7 +8747,9 @@
       <c r="D110" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="E110" s="28"/>
+      <c r="E110" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F110" s="28"/>
       <c r="G110" s="23"/>
       <c r="H110" s="23"/>
@@ -8735,7 +8805,9 @@
       <c r="D112" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="E112" s="28"/>
+      <c r="E112" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F112" s="23" t="s">
         <v>43</v>
       </c>
@@ -8953,7 +9025,9 @@
       <c r="D119" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="E119" s="28"/>
+      <c r="E119" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F119" s="23" t="s">
         <v>43</v>
       </c>
@@ -9061,7 +9135,9 @@
       <c r="D123" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="E123" s="28"/>
+      <c r="E123" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F123" s="23" t="s">
         <v>43</v>
       </c>
@@ -9279,7 +9355,9 @@
       <c r="D130" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="E130" s="28"/>
+      <c r="E130" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F130" s="23" t="s">
         <v>43</v>
       </c>
@@ -9387,7 +9465,9 @@
       <c r="D134" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="E134" s="28"/>
+      <c r="E134" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F134" s="23" t="s">
         <v>43</v>
       </c>
@@ -9511,7 +9591,9 @@
       <c r="D138" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="E138" s="28"/>
+      <c r="E138" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F138" s="23" t="s">
         <v>33</v>
       </c>
@@ -9573,7 +9655,9 @@
       <c r="D140" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="E140" s="28"/>
+      <c r="E140" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F140" s="23" t="s">
         <v>43</v>
       </c>
@@ -9601,7 +9685,9 @@
       <c r="D141" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="E141" s="28"/>
+      <c r="E141" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F141" s="23" t="s">
         <v>43</v>
       </c>
@@ -9629,7 +9715,9 @@
       <c r="D142" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="E142" s="28"/>
+      <c r="E142" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F142" s="23" t="s">
         <v>33</v>
       </c>
@@ -9677,7 +9765,9 @@
       <c r="D144" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="E144" s="28"/>
+      <c r="E144" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F144" s="23" t="s">
         <v>33</v>
       </c>
@@ -9707,7 +9797,9 @@
       <c r="D145" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="E145" s="28"/>
+      <c r="E145" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F145" s="23" t="s">
         <v>43</v>
       </c>
@@ -9735,7 +9827,9 @@
       <c r="D146" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="E146" s="28"/>
+      <c r="E146" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F146" s="23" t="s">
         <v>43</v>
       </c>
@@ -9763,7 +9857,9 @@
       <c r="D147" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="E147" s="28"/>
+      <c r="E147" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F147" s="23" t="s">
         <v>43</v>
       </c>
@@ -12538,7 +12634,9 @@
         <v>32</v>
       </c>
       <c r="D247" s="23"/>
-      <c r="E247" s="28"/>
+      <c r="E247" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F247" s="23" t="s">
         <v>43</v>
       </c>
@@ -13777,7 +13875,9 @@
         <v>32</v>
       </c>
       <c r="D289" s="23"/>
-      <c r="E289" s="28"/>
+      <c r="E289" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F289" s="23" t="s">
         <v>43</v>
       </c>
@@ -14853,7 +14953,9 @@
       <c r="D325" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="E325" s="28"/>
+      <c r="E325" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F325" s="28"/>
       <c r="G325" s="23"/>
       <c r="H325" s="23"/>
@@ -15035,7 +15137,9 @@
       <c r="D331" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="E331" s="28"/>
+      <c r="E331" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F331" s="23" t="s">
         <v>43</v>
       </c>
@@ -15771,7 +15875,9 @@
         <v>32</v>
       </c>
       <c r="D357" s="23"/>
-      <c r="E357" s="28"/>
+      <c r="E357" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F357" s="23" t="s">
         <v>43</v>
       </c>
@@ -16203,7 +16309,9 @@
         <v>32</v>
       </c>
       <c r="D371" s="23"/>
-      <c r="E371" s="28"/>
+      <c r="E371" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F371" s="23" t="s">
         <v>43</v>
       </c>
@@ -16344,7 +16452,9 @@
         <v>32</v>
       </c>
       <c r="D376" s="23"/>
-      <c r="E376" s="28"/>
+      <c r="E376" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F376" s="23" t="s">
         <v>43</v>
       </c>
@@ -16663,7 +16773,9 @@
         <v>32</v>
       </c>
       <c r="D387" s="23"/>
-      <c r="E387" s="28"/>
+      <c r="E387" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F387" s="23" t="s">
         <v>43</v>
       </c>
@@ -16835,7 +16947,9 @@
         <v>32</v>
       </c>
       <c r="D393" s="23"/>
-      <c r="E393" s="28"/>
+      <c r="E393" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F393" s="23" t="s">
         <v>43</v>
       </c>
@@ -17522,7 +17636,9 @@
         <v>32</v>
       </c>
       <c r="D418" s="23"/>
-      <c r="E418" s="28"/>
+      <c r="E418" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F418" s="23" t="s">
         <v>43</v>
       </c>
@@ -18254,7 +18370,9 @@
         <v>32</v>
       </c>
       <c r="D443" s="23"/>
-      <c r="E443" s="28"/>
+      <c r="E443" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F443" s="23" t="s">
         <v>43</v>
       </c>
@@ -18735,7 +18853,9 @@
         <v>32</v>
       </c>
       <c r="D460" s="23"/>
-      <c r="E460" s="28"/>
+      <c r="E460" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F460" s="23" t="s">
         <v>43</v>
       </c>
@@ -19184,7 +19304,9 @@
         <v>32</v>
       </c>
       <c r="D475" s="23"/>
-      <c r="E475" s="28"/>
+      <c r="E475" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F475" s="23" t="s">
         <v>43</v>
       </c>
@@ -19547,7 +19669,9 @@
         <v>32</v>
       </c>
       <c r="D488" s="23"/>
-      <c r="E488" s="28"/>
+      <c r="E488" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F488" s="23" t="s">
         <v>43</v>
       </c>
@@ -20938,7 +21062,9 @@
         <v>32</v>
       </c>
       <c r="D536" s="23"/>
-      <c r="E536" s="28"/>
+      <c r="E536" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F536" s="23" t="s">
         <v>43</v>
       </c>
@@ -21209,7 +21335,9 @@
         <v>32</v>
       </c>
       <c r="D545" s="23"/>
-      <c r="E545" s="28"/>
+      <c r="E545" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F545" s="23" t="s">
         <v>43</v>
       </c>
@@ -21551,7 +21679,9 @@
       <c r="D557" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="E557" s="28"/>
+      <c r="E557" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F557" s="23" t="s">
         <v>33</v>
       </c>
@@ -21579,7 +21709,9 @@
         <v>32</v>
       </c>
       <c r="D558" s="23"/>
-      <c r="E558" s="28"/>
+      <c r="E558" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F558" s="23" t="s">
         <v>43</v>
       </c>
@@ -21605,7 +21737,9 @@
         <v>32</v>
       </c>
       <c r="D559" s="23"/>
-      <c r="E559" s="28"/>
+      <c r="E559" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F559" s="23" t="s">
         <v>33</v>
       </c>
@@ -21631,7 +21765,9 @@
         <v>32</v>
       </c>
       <c r="D560" s="23"/>
-      <c r="E560" s="28"/>
+      <c r="E560" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F560" s="23" t="s">
         <v>43</v>
       </c>
@@ -21657,7 +21793,9 @@
         <v>32</v>
       </c>
       <c r="D561" s="23"/>
-      <c r="E561" s="28"/>
+      <c r="E561" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F561" s="23" t="s">
         <v>33</v>
       </c>
@@ -23546,7 +23684,9 @@
         <v>32</v>
       </c>
       <c r="D631" s="23"/>
-      <c r="E631" s="28"/>
+      <c r="E631" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F631" s="23" t="s">
         <v>43</v>
       </c>
@@ -23732,7 +23872,9 @@
         <v>32</v>
       </c>
       <c r="D638" s="23"/>
-      <c r="E638" s="28"/>
+      <c r="E638" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F638" s="23" t="s">
         <v>43</v>
       </c>
@@ -31798,7 +31940,9 @@
         <v>32</v>
       </c>
       <c r="D955" s="23"/>
-      <c r="E955" s="28"/>
+      <c r="E955" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F955" s="23" t="s">
         <v>43</v>
       </c>
@@ -31825,7 +31969,9 @@
         <v>32</v>
       </c>
       <c r="D956" s="23"/>
-      <c r="E956" s="28"/>
+      <c r="E956" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F956" s="23" t="s">
         <v>43</v>
       </c>
@@ -32171,7 +32317,9 @@
         <v>32</v>
       </c>
       <c r="D968" s="23"/>
-      <c r="E968" s="28"/>
+      <c r="E968" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F968" s="23" t="s">
         <v>43</v>
       </c>
@@ -32198,7 +32346,9 @@
         <v>32</v>
       </c>
       <c r="D969" s="23"/>
-      <c r="E969" s="28"/>
+      <c r="E969" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F969" s="23" t="s">
         <v>43</v>
       </c>
@@ -32312,7 +32462,9 @@
         <v>32</v>
       </c>
       <c r="D973" s="23"/>
-      <c r="E973" s="28"/>
+      <c r="E973" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F973" s="23" t="s">
         <v>43</v>
       </c>
@@ -33184,9 +33336,13 @@
       <c r="B1006" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="C1006" s="28"/>
+      <c r="C1006" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="D1006" s="23"/>
-      <c r="E1006" s="28"/>
+      <c r="E1006" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F1006" s="28"/>
       <c r="G1006" s="23"/>
       <c r="H1006" s="23"/>
@@ -33227,15 +33383,21 @@
       <c r="L1007" s="23"/>
       <c r="M1007" s="23"/>
       <c r="N1007" s="23"/>
-      <c r="O1007" s="25"/>
+      <c r="O1007" s="25" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="1008" customFormat="false" ht="15.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1008" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="C1008" s="28"/>
+      <c r="C1008" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="D1008" s="23"/>
-      <c r="E1008" s="28"/>
+      <c r="E1008" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F1008" s="28"/>
       <c r="G1008" s="23"/>
       <c r="H1008" s="23"/>
@@ -33255,11 +33417,15 @@
       <c r="B1009" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="C1009" s="28"/>
+      <c r="C1009" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="D1009" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="E1009" s="28"/>
+      <c r="E1009" s="23" t="s">
+        <v>59</v>
+      </c>
       <c r="F1009" s="28"/>
       <c r="G1009" s="23"/>
       <c r="H1009" s="23"/>
@@ -33279,9 +33445,13 @@
       <c r="B1010" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="C1010" s="28"/>
+      <c r="C1010" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="D1010" s="23"/>
-      <c r="E1010" s="28"/>
+      <c r="E1010" s="23" t="s">
+        <v>59</v>
+      </c>
       <c r="F1010" s="28"/>
       <c r="G1010" s="23"/>
       <c r="H1010" s="23"/>
@@ -33301,9 +33471,13 @@
       <c r="B1011" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="C1011" s="28"/>
+      <c r="C1011" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="D1011" s="23"/>
-      <c r="E1011" s="28"/>
+      <c r="E1011" s="23" t="s">
+        <v>59</v>
+      </c>
       <c r="F1011" s="28"/>
       <c r="G1011" s="23"/>
       <c r="H1011" s="23"/>
@@ -33323,9 +33497,13 @@
       <c r="B1012" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="C1012" s="28"/>
+      <c r="C1012" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="D1012" s="23"/>
-      <c r="E1012" s="28"/>
+      <c r="E1012" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F1012" s="28"/>
       <c r="G1012" s="23"/>
       <c r="H1012" s="23"/>
@@ -33345,9 +33523,13 @@
       <c r="B1013" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="C1013" s="28"/>
+      <c r="C1013" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="D1013" s="23"/>
-      <c r="E1013" s="28"/>
+      <c r="E1013" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F1013" s="28"/>
       <c r="G1013" s="23"/>
       <c r="H1013" s="23"/>
@@ -33367,9 +33549,13 @@
       <c r="B1014" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="C1014" s="28"/>
+      <c r="C1014" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="D1014" s="23"/>
-      <c r="E1014" s="28"/>
+      <c r="E1014" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F1014" s="28"/>
       <c r="G1014" s="23"/>
       <c r="H1014" s="23"/>
@@ -33389,9 +33575,13 @@
       <c r="B1015" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="C1015" s="28"/>
+      <c r="C1015" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="D1015" s="23"/>
-      <c r="E1015" s="28"/>
+      <c r="E1015" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F1015" s="28"/>
       <c r="G1015" s="23"/>
       <c r="H1015" s="23"/>
@@ -33411,9 +33601,13 @@
       <c r="B1016" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="C1016" s="28"/>
+      <c r="C1016" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="D1016" s="23"/>
-      <c r="E1016" s="28"/>
+      <c r="E1016" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F1016" s="28"/>
       <c r="G1016" s="23"/>
       <c r="H1016" s="23"/>
@@ -35323,7 +35517,9 @@
       </c>
       <c r="C1088" s="28"/>
       <c r="D1088" s="23"/>
-      <c r="E1088" s="28"/>
+      <c r="E1088" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F1088" s="28"/>
       <c r="G1088" s="23"/>
       <c r="H1088" s="23"/>
@@ -35364,7 +35560,9 @@
       <c r="L1089" s="23"/>
       <c r="M1089" s="23"/>
       <c r="N1089" s="23"/>
-      <c r="O1089" s="25"/>
+      <c r="O1089" s="25" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="1090" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1090" s="23" t="s">
@@ -35372,7 +35570,9 @@
       </c>
       <c r="C1090" s="28"/>
       <c r="D1090" s="23"/>
-      <c r="E1090" s="28"/>
+      <c r="E1090" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F1090" s="28"/>
       <c r="G1090" s="23"/>
       <c r="H1090" s="23"/>
@@ -35396,7 +35596,9 @@
       <c r="D1091" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="E1091" s="28"/>
+      <c r="E1091" s="23" t="s">
+        <v>59</v>
+      </c>
       <c r="F1091" s="28"/>
       <c r="G1091" s="23"/>
       <c r="H1091" s="23"/>
@@ -35418,7 +35620,9 @@
       </c>
       <c r="C1092" s="28"/>
       <c r="D1092" s="23"/>
-      <c r="E1092" s="28"/>
+      <c r="E1092" s="23" t="s">
+        <v>59</v>
+      </c>
       <c r="F1092" s="28"/>
       <c r="G1092" s="23"/>
       <c r="H1092" s="23"/>
@@ -35440,7 +35644,9 @@
       </c>
       <c r="C1093" s="28"/>
       <c r="D1093" s="23"/>
-      <c r="E1093" s="28"/>
+      <c r="E1093" s="23" t="s">
+        <v>59</v>
+      </c>
       <c r="F1093" s="28"/>
       <c r="G1093" s="23"/>
       <c r="H1093" s="23"/>
@@ -35462,7 +35668,9 @@
       </c>
       <c r="C1094" s="28"/>
       <c r="D1094" s="23"/>
-      <c r="E1094" s="28"/>
+      <c r="E1094" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F1094" s="28"/>
       <c r="G1094" s="23"/>
       <c r="H1094" s="23"/>
@@ -35484,7 +35692,9 @@
       </c>
       <c r="C1095" s="28"/>
       <c r="D1095" s="23"/>
-      <c r="E1095" s="28"/>
+      <c r="E1095" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F1095" s="28"/>
       <c r="G1095" s="23"/>
       <c r="H1095" s="23"/>
@@ -35506,7 +35716,9 @@
       </c>
       <c r="C1096" s="28"/>
       <c r="D1096" s="23"/>
-      <c r="E1096" s="28"/>
+      <c r="E1096" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F1096" s="28"/>
       <c r="G1096" s="23"/>
       <c r="H1096" s="23"/>
@@ -35528,7 +35740,9 @@
       </c>
       <c r="C1097" s="28"/>
       <c r="D1097" s="23"/>
-      <c r="E1097" s="28"/>
+      <c r="E1097" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F1097" s="28"/>
       <c r="G1097" s="23"/>
       <c r="H1097" s="23"/>
@@ -35550,7 +35764,9 @@
       </c>
       <c r="C1098" s="28"/>
       <c r="D1098" s="23"/>
-      <c r="E1098" s="28"/>
+      <c r="E1098" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F1098" s="28"/>
       <c r="G1098" s="23"/>
       <c r="H1098" s="23"/>
@@ -53537,7 +53753,9 @@
       <c r="D1620" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="E1620" s="28"/>
+      <c r="E1620" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F1620" s="23" t="s">
         <v>977</v>
       </c>
@@ -53589,7 +53807,9 @@
       <c r="D1622" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="E1622" s="28"/>
+      <c r="E1622" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F1622" s="23" t="s">
         <v>977</v>
       </c>
@@ -53613,7 +53833,9 @@
       <c r="D1623" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="E1623" s="28"/>
+      <c r="E1623" s="23" t="s">
+        <v>59</v>
+      </c>
       <c r="F1623" s="23" t="s">
         <v>977</v>
       </c>
@@ -55457,7 +55679,9 @@
       <c r="D1689" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="E1689" s="28"/>
+      <c r="E1689" s="23" t="s">
+        <v>32</v>
+      </c>
       <c r="F1689" s="23" t="s">
         <v>977</v>
       </c>
@@ -55481,7 +55705,9 @@
       <c r="D1690" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="E1690" s="28"/>
+      <c r="E1690" s="23" t="s">
+        <v>59</v>
+      </c>
       <c r="F1690" s="23" t="s">
         <v>977</v>
       </c>

</xml_diff>